<commit_message>
GPLIM-5973 add aggregation data type to Pooled Tube upload
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/PooledTubesTest.xlsx
+++ b/mercury/src/test/resources/testdata/PooledTubesTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="7140" windowWidth="31520" windowHeight="10620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Tube barcode</t>
   </si>
@@ -78,76 +78,82 @@
     <t>PT-JT1</t>
   </si>
   <si>
+    <t>broadinstitute.org:bsp.dev.sample:JT1</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Fragment Size</t>
+  </si>
+  <si>
+    <t>Read Length</t>
+  </si>
+  <si>
+    <t>SM-46IRUT1</t>
+  </si>
+  <si>
+    <t>SM-JT12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>JT041431</t>
+  </si>
+  <si>
+    <t>SM-JT23</t>
+  </si>
+  <si>
+    <t>Illumina_P5-Piwan_P7-Bidih</t>
+  </si>
+  <si>
+    <t>COLLAB-JT04122</t>
+  </si>
+  <si>
+    <t>COLLAB-P-JT04122</t>
+  </si>
+  <si>
+    <t>PT-JT2</t>
+  </si>
+  <si>
+    <t>broadinstitute.org:bsp.dev.sample:JT2</t>
+  </si>
+  <si>
+    <t>SM-46IRUT2</t>
+  </si>
+  <si>
+    <t>Data Analysis Type</t>
+  </si>
+  <si>
+    <t>HybridSelection.Resequencing</t>
+  </si>
+  <si>
+    <t>Data Aggregator</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>UMIs Present</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Aggregation Data Type</t>
+  </si>
+  <si>
+    <t>Exome</t>
+  </si>
+  <si>
+    <t>Jon_Test_3a</t>
+  </si>
+  <si>
+    <t>Jon_Test_4b</t>
+  </si>
+  <si>
     <t>Homo Sapiens</t>
-  </si>
-  <si>
-    <t>broadinstitute.org:bsp.dev.sample:JT1</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Fragment Size</t>
-  </si>
-  <si>
-    <t>Read Length</t>
-  </si>
-  <si>
-    <t>SM-46IRUT1</t>
-  </si>
-  <si>
-    <t>SM-JT12</t>
-  </si>
-  <si>
-    <t>Jon Test 3a</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>JT041431</t>
-  </si>
-  <si>
-    <t>Jon Test 4b</t>
-  </si>
-  <si>
-    <t>SM-JT23</t>
-  </si>
-  <si>
-    <t>Illumina_P5-Piwan_P7-Bidih</t>
-  </si>
-  <si>
-    <t>COLLAB-JT04122</t>
-  </si>
-  <si>
-    <t>COLLAB-P-JT04122</t>
-  </si>
-  <si>
-    <t>PT-JT2</t>
-  </si>
-  <si>
-    <t>broadinstitute.org:bsp.dev.sample:JT2</t>
-  </si>
-  <si>
-    <t>SM-46IRUT2</t>
-  </si>
-  <si>
-    <t>Data Analysis Type</t>
-  </si>
-  <si>
-    <t>HybridSelection.Resequencing</t>
-  </si>
-  <si>
-    <t>Data Aggregator</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>UMIs Present</t>
-  </si>
-  <si>
-    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -603,9 +609,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -628,10 +636,11 @@
     <col min="17" max="17" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.83203125" style="2"/>
+    <col min="20" max="20" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1">
+    <row r="1" spans="1:20" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,36 +681,39 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>13</v>
@@ -719,13 +731,13 @@
         <v>17</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="N2" s="2">
         <v>0.6</v>
@@ -737,63 +749,66 @@
         <v>4</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="P3" s="2">
         <v>2</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="Q5" s="5"/>
     </row>
   </sheetData>

</xml_diff>